<commit_message>
BE LTd - Account number Expo Fix
</commit_message>
<xml_diff>
--- a/BELtd_HDFC_UTR_Windows/Data/Config.xlsx
+++ b/BELtd_HDFC_UTR_Windows/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BRADSOL-User\Documents\GitHub\biologicale\BELtd_HDFC_UTR_Windows\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48FFD78-185F-41FC-8C6B-18A6755AC395}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC9AD84-7F5C-4093-AD37-B6677322C556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -224,9 +224,6 @@
     <t>AttachmentNotFound_MailSubject</t>
   </si>
   <si>
-    <t>MM-dd-yyyy</t>
-  </si>
-  <si>
     <t>NoPDFFoundInTheEmail_MailSubject</t>
   </si>
   <si>
@@ -473,9 +470,6 @@
     <t>VendorPaymentFileSubjectFilter</t>
   </si>
   <si>
-    <t>VendorFileSavingPath</t>
-  </si>
-  <si>
     <t>VendorPaymentsFileName</t>
   </si>
   <si>
@@ -554,12 +548,6 @@
     <t xml:space="preserve">HDFC UTR Automation - Execution Completed </t>
   </si>
   <si>
-    <t>&lt;p&gt;Hello Team, &lt;/p&gt;
-&lt;p&gt;This is to notify you that our BOT completed the process for HDFC UTR Automation with errors. &lt;/p&gt;
-&lt;p&gt;Thanks &amp; Regards &lt;/p&gt;
-&lt;p&gt;BE Ltd.&lt;/p&gt;</t>
-  </si>
-  <si>
     <t>Bot_Ending_Mail_Subject_Success</t>
   </si>
   <si>
@@ -696,6 +684,19 @@
   </si>
   <si>
     <t>Bank A/C No.</t>
+  </si>
+  <si>
+    <t>dd-MM-yyyy</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Hello Team, &lt;/p&gt;
+&lt;p&gt;This is to notify you that our BOT completed the process for HDFC UTR Automation with below error. &lt;/p&gt;
+&lt;p&gt;"{0}"&lt;/p&gt;
+&lt;p&gt;Thanks &amp; Regards &lt;/p&gt;
+&lt;p&gt;BE Ltd.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>VendorFileSavingPath</t>
   </si>
 </sst>
 </file>
@@ -763,35 +764,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="12">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1109,10 +1104,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1039"/>
+  <dimension ref="A1:Z1040"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -1158,407 +1153,391 @@
       <c r="Z1" s="1"/>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A3" s="4" t="s">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A4" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>181</v>
+      <c r="B4" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>135</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="B6" s="4"/>
-    </row>
+        <v>134</v>
+      </c>
+      <c r="B5" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" t="s">
         <v>92</v>
-      </c>
-      <c r="B8" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>193</v>
-      </c>
-      <c r="B9" s="15" t="s">
-        <v>195</v>
+        <v>190</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>204</v>
-      </c>
-      <c r="B10" s="15" t="s">
-        <v>205</v>
+        <v>201</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>138</v>
+        <v>205</v>
       </c>
       <c r="B12" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>90</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" t="s">
-        <v>194</v>
-      </c>
-      <c r="B15" s="15" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A17" t="s">
-        <v>137</v>
-      </c>
-      <c r="B17" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B15" s="11" t="s">
         <v>192</v>
       </c>
     </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="B16" s="11"/>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B18" s="9"/>
-    </row>
-    <row r="19" spans="1:3" ht="15" customHeight="1">
-      <c r="A19" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="B19" s="9"/>
-    </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A20" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>143</v>
-      </c>
+      <c r="A18" t="s">
+        <v>136</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="B19" s="6"/>
+    </row>
+    <row r="20" spans="1:3" ht="15" customHeight="1">
+      <c r="A20" t="s">
+        <v>140</v>
+      </c>
+      <c r="B20" s="6"/>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A21" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="B21" s="10">
+      <c r="A21" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="B22" s="7">
         <v>-30</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="15" customHeight="1">
-      <c r="A22" s="4" t="s">
+    <row r="23" spans="1:3" ht="15" customHeight="1">
+      <c r="A23" t="s">
+        <v>128</v>
+      </c>
+      <c r="B23" t="s">
         <v>129</v>
       </c>
-      <c r="B22" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15" customHeight="1">
-      <c r="A23" s="4"/>
-    </row>
-    <row r="24" spans="1:3" ht="15" customHeight="1">
-      <c r="A24" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+    </row>
+    <row r="25" spans="1:3" ht="15" customHeight="1">
       <c r="A25" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" t="s">
-        <v>53</v>
+        <v>147</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>151</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" t="s">
+        <v>149</v>
+      </c>
+      <c r="B27" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A31" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" t="s">
+        <v>180</v>
+      </c>
+      <c r="C31" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A32" t="s">
+        <v>77</v>
+      </c>
+      <c r="B32" t="s">
+        <v>181</v>
+      </c>
+      <c r="C32" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A33" t="s">
+        <v>113</v>
+      </c>
+      <c r="B33" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="36" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A36" t="s">
+        <v>125</v>
+      </c>
+      <c r="B36" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A28" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B28" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C28" s="4"/>
-    </row>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="4"/>
-    </row>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A30" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B30" s="4" t="s">
+    <row r="37" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A37" t="s">
+        <v>126</v>
+      </c>
+      <c r="B37" t="s">
         <v>183</v>
       </c>
-      <c r="C30" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A31" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B31" s="4" t="s">
+    </row>
+    <row r="38" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A38" t="s">
+        <v>154</v>
+      </c>
+      <c r="B38" t="s">
         <v>184</v>
       </c>
-      <c r="C31" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A32" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-    </row>
-    <row r="35" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A35" t="s">
-        <v>126</v>
-      </c>
-      <c r="B35" s="4" t="s">
+    </row>
+    <row r="39" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A39" t="s">
+        <v>172</v>
+      </c>
+      <c r="B39" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A36" t="s">
-        <v>127</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A37" t="s">
-        <v>156</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A38" t="s">
+    <row r="40" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A41" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A42" t="s">
+        <v>57</v>
+      </c>
+      <c r="B42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B43" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A44" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A45" t="s">
+        <v>60</v>
+      </c>
+      <c r="B45" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A46" t="s">
+        <v>142</v>
+      </c>
+      <c r="B46" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A47" t="s">
+        <v>143</v>
+      </c>
+      <c r="B47" t="s">
         <v>175</v>
       </c>
-      <c r="B38" s="4" t="s">
+    </row>
+    <row r="48" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="49" spans="1:3" ht="14.4">
+      <c r="A49" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49" s="3"/>
+    </row>
+    <row r="50" spans="1:3" ht="14.4">
+      <c r="C50" s="3"/>
+    </row>
+    <row r="51" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A51" t="s">
+        <v>80</v>
+      </c>
+      <c r="B51" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="40" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A40" t="s">
-        <v>52</v>
-      </c>
-      <c r="B40" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A41" t="s">
-        <v>57</v>
-      </c>
-      <c r="B41" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A42" t="s">
-        <v>58</v>
-      </c>
-      <c r="B42" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A43" t="s">
-        <v>59</v>
-      </c>
-      <c r="B43" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A44" t="s">
-        <v>60</v>
-      </c>
-      <c r="B44" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A45" t="s">
-        <v>144</v>
-      </c>
-      <c r="B45" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A46" t="s">
-        <v>145</v>
-      </c>
-      <c r="B46" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="48" spans="1:3" ht="14.4">
-      <c r="A48" t="s">
-        <v>51</v>
-      </c>
-      <c r="B48" t="s">
-        <v>50</v>
-      </c>
-      <c r="C48" s="3"/>
-    </row>
-    <row r="49" spans="1:3" ht="14.4">
-      <c r="C49" s="3"/>
-    </row>
-    <row r="50" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A50" s="4" t="s">
+    <row r="52" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="53" spans="1:3" ht="14.25" customHeight="1">
+      <c r="B53" s="6"/>
+    </row>
+    <row r="54" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="55" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A55" t="s">
         <v>81</v>
       </c>
-      <c r="B50" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A51" s="4"/>
-    </row>
-    <row r="52" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B52" s="9"/>
-    </row>
-    <row r="53" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="54" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A54" t="s">
-        <v>82</v>
-      </c>
-      <c r="B54" s="7">
+      <c r="B55" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B55" s="7"/>
-    </row>
     <row r="56" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A56" t="s">
-        <v>140</v>
-      </c>
-      <c r="B56" s="7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="14.4">
-      <c r="B57" s="4"/>
-      <c r="C57" s="3"/>
-    </row>
-    <row r="58" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A58" t="s">
-        <v>69</v>
-      </c>
-      <c r="B58" t="s">
-        <v>70</v>
-      </c>
+      <c r="B56" s="5"/>
+    </row>
+    <row r="57" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A57" t="s">
+        <v>138</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="14.4">
+      <c r="C58" s="3"/>
     </row>
     <row r="59" spans="1:3" ht="14.25" customHeight="1">
       <c r="A59" t="s">
+        <v>68</v>
+      </c>
+      <c r="B59" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A60" t="s">
+        <v>71</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="14.25" customHeight="1">
+      <c r="B61" s="4"/>
+    </row>
+    <row r="62" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A62" t="s">
         <v>72</v>
       </c>
-      <c r="B59" s="5" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B60" s="5"/>
-    </row>
-    <row r="61" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A61" s="4" t="s">
+      <c r="B62" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A63" t="s">
         <v>73</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B63" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A62" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B62" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" ht="14.4">
-      <c r="B64" s="4"/>
-    </row>
-    <row r="65" ht="14.25" customHeight="1"/>
+    <row r="65" ht="14.4"/>
     <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.4"/>
-    <row r="68" ht="14.25" customHeight="1"/>
+    <row r="67" ht="14.25" customHeight="1"/>
+    <row r="68" ht="14.4"/>
     <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.4"/>
-    <row r="71" ht="14.25" customHeight="1"/>
+    <row r="70" ht="14.25" customHeight="1"/>
+    <row r="71" ht="14.4"/>
     <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.4"/>
+    <row r="73" ht="14.25" customHeight="1"/>
     <row r="74" ht="14.4"/>
-    <row r="75" ht="14.25" customHeight="1"/>
+    <row r="75" ht="14.4"/>
     <row r="76" ht="14.25" customHeight="1"/>
     <row r="77" ht="14.25" customHeight="1"/>
     <row r="78" ht="14.25" customHeight="1"/>
@@ -2523,13 +2502,14 @@
     <row r="1037" ht="14.25" customHeight="1"/>
     <row r="1038" ht="14.25" customHeight="1"/>
     <row r="1039" ht="14.25" customHeight="1"/>
+    <row r="1040" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <hyperlinks>
-    <hyperlink ref="B20" r:id="rId1" xr:uid="{BE3800E5-4AA0-48DE-8F2D-931BEB786182}"/>
-    <hyperlink ref="B61" r:id="rId2" xr:uid="{F19909F1-85DB-4E23-B380-9D1AF9BD4AB0}"/>
-    <hyperlink ref="B59" r:id="rId3" xr:uid="{E8EB690E-788E-469D-948B-38D2F80252DF}"/>
-    <hyperlink ref="B62" r:id="rId4" xr:uid="{D578C2D8-D83E-4A95-AC4B-85AD1BF7983A}"/>
+    <hyperlink ref="B21" r:id="rId1" xr:uid="{BE3800E5-4AA0-48DE-8F2D-931BEB786182}"/>
+    <hyperlink ref="B62" r:id="rId2" xr:uid="{F19909F1-85DB-4E23-B380-9D1AF9BD4AB0}"/>
+    <hyperlink ref="B60" r:id="rId3" xr:uid="{E8EB690E-788E-469D-948B-38D2F80252DF}"/>
+    <hyperlink ref="B63" r:id="rId4" xr:uid="{D578C2D8-D83E-4A95-AC4B-85AD1BF7983A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
@@ -2540,8 +2520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z1022"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B80" sqref="B80"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -2727,19 +2707,17 @@
       <c r="A19" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="4" t="s">
-        <v>84</v>
+      <c r="B19" t="s">
+        <v>83</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.4">
-      <c r="B20" s="4"/>
       <c r="C20" s="3"/>
     </row>
     <row r="35" spans="1:3" ht="14.4">
-      <c r="B35" s="4"/>
       <c r="C35" s="3"/>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1">
@@ -2755,316 +2733,316 @@
         <v>62</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="39" spans="1:3" ht="14.25" customHeight="1">
       <c r="A39" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B39" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="14.25" customHeight="1">
       <c r="A40" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="42" spans="1:3" ht="14.25" customHeight="1">
       <c r="A42" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B42" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="14.25" customHeight="1">
       <c r="A43" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>162</v>
+        <v>204</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="14.25" customHeight="1">
       <c r="A45" t="s">
-        <v>153</v>
-      </c>
-      <c r="B45" s="8" t="s">
-        <v>172</v>
+        <v>151</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="14.25" customHeight="1">
       <c r="A46" t="s">
-        <v>154</v>
-      </c>
-      <c r="B46" s="8" t="s">
-        <v>155</v>
+        <v>152</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="14.25" customHeight="1">
-      <c r="B47" s="8"/>
+      <c r="B47" s="2"/>
     </row>
     <row r="48" spans="1:3" ht="14.25" customHeight="1">
       <c r="A48" t="s">
-        <v>171</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>173</v>
+        <v>168</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="14.25" customHeight="1">
       <c r="A49" t="s">
-        <v>170</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>174</v>
+        <v>167</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="51" spans="1:2" ht="14.25" customHeight="1">
       <c r="A51" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B51" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="14.25" customHeight="1">
       <c r="A52" t="s">
-        <v>96</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>116</v>
+        <v>95</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="54" spans="1:2" ht="14.25" customHeight="1">
       <c r="A54" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="14.25" customHeight="1">
       <c r="A55" t="s">
-        <v>98</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>121</v>
+        <v>97</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="57" spans="1:2" ht="14.25" customHeight="1">
       <c r="A57" t="s">
-        <v>99</v>
-      </c>
-      <c r="B57" s="8" t="s">
-        <v>94</v>
+        <v>98</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="14.25" customHeight="1">
       <c r="A58" t="s">
-        <v>100</v>
-      </c>
-      <c r="B58" s="8" t="s">
-        <v>122</v>
+        <v>99</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="60" spans="1:2" ht="14.25" customHeight="1">
       <c r="A60" t="s">
-        <v>101</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>94</v>
+        <v>100</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="14.25" customHeight="1">
       <c r="A61" t="s">
-        <v>102</v>
-      </c>
-      <c r="B61" s="8" t="s">
-        <v>123</v>
+        <v>101</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="63" spans="1:2" ht="14.25" customHeight="1">
       <c r="A63" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B63" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="14.25" customHeight="1">
       <c r="A64" t="s">
-        <v>104</v>
-      </c>
-      <c r="B64" s="8" t="s">
-        <v>124</v>
+        <v>103</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="66" spans="1:2" ht="14.25" customHeight="1">
       <c r="A66" t="s">
-        <v>105</v>
-      </c>
-      <c r="B66" s="8" t="s">
-        <v>94</v>
+        <v>104</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="14.25" customHeight="1">
       <c r="A67" t="s">
-        <v>106</v>
-      </c>
-      <c r="B67" s="8" t="s">
-        <v>118</v>
+        <v>105</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="69" spans="1:2" ht="14.25" customHeight="1">
       <c r="A69" t="s">
+        <v>106</v>
+      </c>
+      <c r="B69" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="B69" s="8" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="14.25" customHeight="1">
       <c r="A70" t="s">
-        <v>117</v>
-      </c>
-      <c r="B70" s="8" t="s">
-        <v>152</v>
+        <v>116</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="72" spans="1:2" ht="14.25" customHeight="1">
       <c r="A72" t="s">
+        <v>110</v>
+      </c>
+      <c r="B72" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="B72" s="8" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="14.25" customHeight="1">
       <c r="A73" t="s">
-        <v>113</v>
-      </c>
-      <c r="B73" s="8" t="s">
-        <v>125</v>
+        <v>112</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="14.25" customHeight="1">
-      <c r="B74" s="8"/>
+      <c r="B74" s="2"/>
     </row>
     <row r="75" spans="1:2" ht="14.25" customHeight="1">
       <c r="A75" t="s">
-        <v>131</v>
-      </c>
-      <c r="B75" s="8" t="s">
-        <v>133</v>
+        <v>130</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="14.25" customHeight="1">
       <c r="A76" t="s">
-        <v>132</v>
-      </c>
-      <c r="B76" s="8" t="s">
-        <v>134</v>
+        <v>131</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="14.25" customHeight="1">
-      <c r="B77" s="8"/>
+      <c r="B77" s="2"/>
     </row>
     <row r="78" spans="1:2" ht="14.25" customHeight="1">
       <c r="A78" t="s">
+        <v>155</v>
+      </c>
+      <c r="B78" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="B78" s="8" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="14.25" customHeight="1">
       <c r="A79" t="s">
+        <v>156</v>
+      </c>
+      <c r="B79" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B79" s="8" t="s">
-        <v>160</v>
-      </c>
     </row>
     <row r="80" spans="1:2" ht="14.25" customHeight="1">
-      <c r="B80" s="8"/>
+      <c r="B80" s="2"/>
     </row>
     <row r="81" spans="1:2" ht="14.25" customHeight="1">
       <c r="A81" t="s">
-        <v>196</v>
-      </c>
-      <c r="B81" s="8" t="s">
-        <v>198</v>
+        <v>193</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="14.25" customHeight="1">
       <c r="A82" t="s">
-        <v>197</v>
-      </c>
-      <c r="B82" s="8" t="s">
-        <v>199</v>
+        <v>194</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="14.25" customHeight="1">
-      <c r="B83" s="8"/>
+      <c r="B83" s="2"/>
     </row>
     <row r="84" spans="1:2" ht="14.25" customHeight="1">
       <c r="A84" t="s">
-        <v>200</v>
-      </c>
-      <c r="B84" s="8" t="s">
-        <v>202</v>
+        <v>197</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="14.25" customHeight="1">
       <c r="A85" t="s">
-        <v>201</v>
-      </c>
-      <c r="B85" s="8" t="s">
-        <v>203</v>
+        <v>198</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="14.25" customHeight="1">
-      <c r="B86" s="8"/>
+      <c r="B86" s="2"/>
     </row>
     <row r="87" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="88" spans="1:2" ht="14.25" customHeight="1">
       <c r="A88" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B88" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="14.25" customHeight="1">
       <c r="A89" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B89" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="14.25" customHeight="1">
       <c r="A90" t="s">
-        <v>167</v>
-      </c>
-      <c r="B90" s="14" t="s">
-        <v>176</v>
+        <v>164</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="91" spans="1:2" ht="14.25" customHeight="1"/>
@@ -3073,50 +3051,50 @@
       <c r="A93" t="s">
         <v>65</v>
       </c>
-      <c r="B93" s="8" t="s">
-        <v>109</v>
+      <c r="B93" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="94" spans="1:2" ht="14.25" customHeight="1">
       <c r="A94" t="s">
         <v>64</v>
       </c>
-      <c r="B94" s="8" t="s">
-        <v>119</v>
+      <c r="B94" s="2" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="95" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="96" spans="1:2" ht="14.25" customHeight="1">
       <c r="A96" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B96" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="97" spans="1:2" ht="14.25" customHeight="1">
       <c r="A97" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="98" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="99" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="100" spans="1:2" s="12" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A100" s="12" t="s">
+    <row r="100" spans="1:2" s="9" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A100" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B100" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B100" s="12" t="s">
+    </row>
+    <row r="101" spans="1:2" s="9" customFormat="1" ht="14.25" customHeight="1">
+      <c r="A101" s="9" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" s="12" customFormat="1" ht="14.25" customHeight="1">
-      <c r="A101" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="B101" s="13">
+      <c r="B101" s="10">
         <v>587</v>
       </c>
     </row>

</xml_diff>